<commit_message>
Commit conectividad extremo a extremo
</commit_message>
<xml_diff>
--- a/CheckLis.xlsx
+++ b/CheckLis.xlsx
@@ -655,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -771,14 +771,14 @@
     <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -792,6 +792,9 @@
     </xf>
     <xf borderId="6" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3758,11 +3761,13 @@
         <v>7.0</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="41"/>
+      <c r="F16" s="38">
+        <v>3.0</v>
+      </c>
       <c r="G16" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="42"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -3785,14 +3790,16 @@
     <row r="17">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="1">
         <v>10.0</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="43">
+        <v>3.0</v>
+      </c>
       <c r="G17" s="39" t="s">
         <v>34</v>
       </c>
@@ -4122,9 +4129,9 @@
         <v>8.0</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="41"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="45"/>
-      <c r="H28" s="42"/>
+      <c r="H28" s="41"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
@@ -4334,8 +4341,8 @@
         <v>10.0</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="41"/>
-      <c r="H35" s="42"/>
+      <c r="F35" s="49"/>
+      <c r="H35" s="41"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
@@ -4411,12 +4418,12 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="50"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="11"/>
@@ -4495,10 +4502,10 @@
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="53"/>
+      <c r="D41" s="54"/>
       <c r="E41" s="14"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
@@ -4522,15 +4529,15 @@
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="55">
+      <c r="D42" s="56">
         <v>3.0</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="41"/>
-      <c r="H42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="49"/>
+      <c r="H42" s="58"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -4553,15 +4560,15 @@
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="55">
+      <c r="D43" s="56">
         <v>3.0</v>
       </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="41"/>
-      <c r="H43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="49"/>
+      <c r="H43" s="58"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
@@ -4584,7 +4591,7 @@
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="56"/>
+      <c r="C44" s="57"/>
       <c r="D44" s="12"/>
       <c r="E44" s="11"/>
       <c r="I44" s="11"/>
@@ -4611,7 +4618,7 @@
       <c r="C45" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="53"/>
+      <c r="D45" s="54"/>
       <c r="E45" s="14"/>
       <c r="F45" s="11"/>
       <c r="H45" s="11"/>
@@ -4644,8 +4651,8 @@
         <v>10.0</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="41"/>
-      <c r="H46" s="42"/>
+      <c r="F46" s="49"/>
+      <c r="H46" s="41"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -4675,8 +4682,8 @@
         <v>5.0</v>
       </c>
       <c r="E47" s="1"/>
-      <c r="F47" s="41"/>
-      <c r="H47" s="42"/>
+      <c r="F47" s="49"/>
+      <c r="H47" s="41"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
@@ -4699,7 +4706,7 @@
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="56"/>
+      <c r="C48" s="57"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="13"/>
@@ -4762,8 +4769,8 @@
         <v>5.0</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="F50" s="41"/>
-      <c r="H50" s="42"/>
+      <c r="F50" s="49"/>
+      <c r="H50" s="41"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
@@ -4793,8 +4800,8 @@
         <v>2.0</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="F51" s="41"/>
-      <c r="H51" s="42"/>
+      <c r="F51" s="49"/>
+      <c r="H51" s="41"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
@@ -4880,8 +4887,8 @@
         <v>3.0</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="F54" s="41"/>
-      <c r="H54" s="42"/>
+      <c r="F54" s="49"/>
+      <c r="H54" s="41"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
@@ -4911,8 +4918,8 @@
         <v>3.0</v>
       </c>
       <c r="E55" s="1"/>
-      <c r="F55" s="41"/>
-      <c r="H55" s="42"/>
+      <c r="F55" s="49"/>
+      <c r="H55" s="41"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
@@ -4942,8 +4949,8 @@
         <v>3.0</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="41"/>
-      <c r="H56" s="42"/>
+      <c r="F56" s="49"/>
+      <c r="H56" s="41"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
@@ -5047,10 +5054,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="11"/>
-      <c r="B60" s="59" t="s">
+      <c r="B60" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="60"/>
+      <c r="C60" s="61"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="13"/>
@@ -5131,15 +5138,15 @@
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="61" t="s">
+      <c r="C63" s="62" t="s">
         <v>64</v>
       </c>
       <c r="D63" s="1">
         <v>2.0</v>
       </c>
       <c r="E63" s="1"/>
-      <c r="F63" s="41"/>
-      <c r="H63" s="57"/>
+      <c r="F63" s="49"/>
+      <c r="H63" s="58"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
       <c r="K63" s="11"/>
@@ -5169,9 +5176,9 @@
         <v>2.0</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="41"/>
+      <c r="F64" s="49"/>
       <c r="G64" s="11"/>
-      <c r="H64" s="42"/>
+      <c r="H64" s="41"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>
@@ -5277,10 +5284,10 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="11"/>
-      <c r="B68" s="62" t="s">
+      <c r="B68" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="63"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="12"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -5342,8 +5349,8 @@
         <v>5.0</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="F70" s="41"/>
-      <c r="H70" s="42"/>
+      <c r="F70" s="49"/>
+      <c r="H70" s="41"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
@@ -5373,8 +5380,8 @@
         <v>5.0</v>
       </c>
       <c r="E71" s="1"/>
-      <c r="F71" s="41"/>
-      <c r="H71" s="42"/>
+      <c r="F71" s="49"/>
+      <c r="H71" s="41"/>
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
@@ -5404,8 +5411,8 @@
         <v>5.0</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="41"/>
-      <c r="H72" s="42"/>
+      <c r="F72" s="49"/>
+      <c r="H72" s="41"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11" t="s">
         <v>68</v>
@@ -5460,11 +5467,11 @@
       <c r="C74" s="46"/>
       <c r="D74" s="12"/>
       <c r="E74" s="11"/>
-      <c r="F74" s="64">
+      <c r="F74" s="65">
         <f>SUM(F15:F72)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
-      <c r="H74" s="64">
+      <c r="H74" s="65">
         <f>SUM(H15:H72)</f>
         <v>0</v>
       </c>
@@ -5552,7 +5559,7 @@
       <c r="D77" s="12"/>
       <c r="E77" s="11"/>
       <c r="F77" s="13"/>
-      <c r="H77" s="65"/>
+      <c r="H77" s="66"/>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
@@ -5602,9 +5609,9 @@
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="67"/>
-      <c r="E79" s="66"/>
+      <c r="C79" s="67"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="67"/>
       <c r="F79" s="13"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
@@ -5683,9 +5690,9 @@
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="67"/>
-      <c r="E82" s="68"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="69"/>
       <c r="F82" s="13"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
@@ -13168,13 +13175,13 @@
       <c r="B7" s="1">
         <v>1.0</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="70" t="s">
         <v>24</v>
       </c>
     </row>
@@ -13182,25 +13189,25 @@
       <c r="B8" s="1">
         <v>2.0</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="9">
       <c r="B9" s="1">
         <v>3.0</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
     </row>
     <row r="10">
       <c r="B10" s="1">
         <v>4.0</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -14208,7 +14215,7 @@
   </cols>
   <sheetData>
     <row r="10">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="72" t="s">
         <v>76</v>
       </c>
     </row>
@@ -14252,7 +14259,7 @@
         <v>81</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="73" t="s">
         <v>82</v>
       </c>
     </row>
@@ -15338,28 +15345,28 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="76" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="74" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="74" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Conectividad de extremo a extremo
</commit_message>
<xml_diff>
--- a/CheckLis.xlsx
+++ b/CheckLis.xlsx
@@ -3762,7 +3762,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="38">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="G16" s="39" t="s">
         <v>34</v>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="43">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="G17" s="39" t="s">
         <v>34</v>
@@ -5469,7 +5469,7 @@
       <c r="E74" s="11"/>
       <c r="F74" s="65">
         <f>SUM(F15:F72)</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="H74" s="65">
         <f>SUM(H15:H72)</f>

</xml_diff>

<commit_message>
Caso de estudio terminado
</commit_message>
<xml_diff>
--- a/CheckLis.xlsx
+++ b/CheckLis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
   <si>
     <t>#Tab</t>
   </si>
@@ -340,6 +340,12 @@
     <t>Quitar ip de la interfaz</t>
   </si>
   <si>
+    <t xml:space="preserve">DNS no encontraba servidor </t>
+  </si>
+  <si>
+    <t>Ingresar la direccion del servidor DNS en el servidor DHCP</t>
+  </si>
+  <si>
     <t>Lessson Learned</t>
   </si>
   <si>
@@ -347,6 +353,9 @@
   </si>
   <si>
     <t>Estrategía Utilizada para solucionar el problema</t>
+  </si>
+  <si>
+    <t>https://github.com/OrtizAxel/Caso-de-estudio.git</t>
   </si>
   <si>
     <t>Que me funciono y lo volveré a repetir</t>
@@ -388,9 +397,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>https://github.com/OrtizAxel/Caso-de-estudio.git</t>
-  </si>
-  <si>
     <t>GitHub</t>
   </si>
   <si>
@@ -404,7 +410,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -513,6 +519,12 @@
     <font>
       <b/>
       <sz val="16.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -864,9 +876,6 @@
     <xf borderId="10" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="1" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,11 +916,14 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyFont="1"/>
@@ -4866,7 +4878,12 @@
         <v>5.0</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="F50" s="60"/>
+      <c r="F50" s="38">
+        <v>5.0</v>
+      </c>
+      <c r="G50" s="49">
+        <v>1.0</v>
+      </c>
       <c r="H50" s="41"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
@@ -4897,7 +4914,12 @@
         <v>2.0</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="F51" s="60"/>
+      <c r="F51" s="38">
+        <v>2.0</v>
+      </c>
+      <c r="G51" s="49">
+        <v>1.0</v>
+      </c>
       <c r="H51" s="41"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
@@ -4984,7 +5006,9 @@
         <v>3.0</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="F54" s="38"/>
+      <c r="F54" s="38">
+        <v>3.0</v>
+      </c>
       <c r="G54" s="49">
         <v>1.0</v>
       </c>
@@ -5018,7 +5042,9 @@
         <v>3.0</v>
       </c>
       <c r="E55" s="1"/>
-      <c r="F55" s="60"/>
+      <c r="F55" s="38">
+        <v>3.0</v>
+      </c>
       <c r="G55" s="49">
         <v>1.0</v>
       </c>
@@ -5052,7 +5078,9 @@
         <v>3.0</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="60"/>
+      <c r="F56" s="38">
+        <v>3.0</v>
+      </c>
       <c r="G56" s="49">
         <v>1.0</v>
       </c>
@@ -5160,10 +5188,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="11"/>
-      <c r="B60" s="61" t="s">
+      <c r="B60" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="62"/>
+      <c r="C60" s="61"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="13"/>
@@ -5244,7 +5272,7 @@
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="63" t="s">
+      <c r="C63" s="62" t="s">
         <v>64</v>
       </c>
       <c r="D63" s="1">
@@ -5287,8 +5315,10 @@
         <v>2.0</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="64">
+      <c r="F64" s="38">
+        <v>2.0</v>
+      </c>
+      <c r="G64" s="63">
         <v>2.0</v>
       </c>
       <c r="H64" s="41"/>
@@ -5397,10 +5427,10 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="11"/>
-      <c r="B68" s="65" t="s">
+      <c r="B68" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="66"/>
+      <c r="C68" s="65"/>
       <c r="D68" s="12"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -5462,7 +5492,9 @@
         <v>5.0</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="F70" s="60"/>
+      <c r="F70" s="38">
+        <v>5.0</v>
+      </c>
       <c r="G70" s="49" t="s">
         <v>68</v>
       </c>
@@ -5496,7 +5528,9 @@
         <v>5.0</v>
       </c>
       <c r="E71" s="1"/>
-      <c r="F71" s="60"/>
+      <c r="F71" s="38">
+        <v>5.0</v>
+      </c>
       <c r="G71" s="49" t="s">
         <v>68</v>
       </c>
@@ -5591,11 +5625,11 @@
       <c r="C74" s="46"/>
       <c r="D74" s="12"/>
       <c r="E74" s="11"/>
-      <c r="F74" s="67">
+      <c r="F74" s="66">
         <f>SUM(F15:F72)</f>
-        <v>72</v>
-      </c>
-      <c r="H74" s="67">
+        <v>100</v>
+      </c>
+      <c r="H74" s="66">
         <f>SUM(H15:H72)</f>
         <v>0</v>
       </c>
@@ -5621,7 +5655,7 @@
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="11"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="64" t="s">
+      <c r="C75" s="63" t="s">
         <v>18</v>
       </c>
       <c r="D75" s="12"/>
@@ -5685,7 +5719,7 @@
       <c r="D77" s="12"/>
       <c r="E77" s="11"/>
       <c r="F77" s="13"/>
-      <c r="H77" s="68"/>
+      <c r="H77" s="67"/>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
@@ -5735,9 +5769,9 @@
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="69"/>
-      <c r="D79" s="70"/>
-      <c r="E79" s="69"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="69"/>
+      <c r="E79" s="68"/>
       <c r="F79" s="13"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
@@ -5816,9 +5850,9 @@
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="71"/>
-      <c r="D82" s="70"/>
-      <c r="E82" s="71"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="70"/>
       <c r="F82" s="13"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
@@ -13301,83 +13335,97 @@
       <c r="B7" s="1">
         <v>1.0</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="71" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="73">
+      <c r="B8" s="72">
         <v>2.0</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="71" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="73">
+      <c r="B9" s="72">
         <v>3.0</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="71" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="73">
+      <c r="B10" s="72">
         <v>4.0</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="71" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="73">
+      <c r="B11" s="72">
         <v>5.0</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="71" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="74">
+      <c r="B12" s="73">
         <v>6.0</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="73">
+        <v>7.0</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="74" t="s">
         <v>82</v>
       </c>
     </row>
@@ -14387,13 +14435,13 @@
   </cols>
   <sheetData>
     <row r="10">
-      <c r="B10" s="76" t="s">
-        <v>89</v>
+      <c r="B10" s="75" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11">
       <c r="I11" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12">
@@ -14401,16 +14449,18 @@
         <v>1.0</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="12">
         <v>2.0</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D13" s="10"/>
     </row>
@@ -14419,7 +14469,7 @@
         <v>3.0</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D14" s="10"/>
     </row>
@@ -14428,11 +14478,11 @@
         <v>4.0</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D15" s="10"/>
       <c r="G15" s="77" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16">
@@ -14447,7 +14497,7 @@
         <v>1.0</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10"/>
     </row>
@@ -14456,7 +14506,7 @@
         <v>2.0</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -14465,7 +14515,7 @@
         <v>3.0</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D20" s="10"/>
     </row>
@@ -15458,10 +15508,13 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D12"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15481,7 +15534,7 @@
   <sheetData>
     <row r="3">
       <c r="B3" s="11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
@@ -15489,7 +15542,7 @@
         <v>1.0</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
@@ -15497,7 +15550,7 @@
         <v>2.0</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
@@ -15505,7 +15558,7 @@
         <v>3.0</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
@@ -15513,41 +15566,41 @@
         <v>4.0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="78" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I8" s="80" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="78" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="78" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="78" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Final con lessons learned
</commit_message>
<xml_diff>
--- a/CheckLis.xlsx
+++ b/CheckLis.xlsx
@@ -1599,11 +1599,39 @@
     <xdr:ext cx="4972050" cy="1971675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7134225" cy="4762500"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>